<commit_message>
update experiment results about topic num of v4
</commit_message>
<xml_diff>
--- a/v4/v4_standard/v4_softmax_temper_regression.xlsx
+++ b/v4/v4_standard/v4_softmax_temper_regression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\master\ensemble_github\experimental_data\v4\v4_standard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B424D8-7D73-481E-B7FA-ACFFB7B77960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08833C9D-2467-453C-8376-E81BA24FC31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="330" windowWidth="21570" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="930" windowWidth="21570" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1230,7 +1230,7 @@
   <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>